<commit_message>
Tratando termos banidos, termos de busca, preços e ajuste na base de dados
</commit_message>
<xml_diff>
--- a/buscas.xlsx
+++ b/buscas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Python\Downloads\Projeto 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bulllasa-my.sharepoint.com/personal/gabriel_souza_bullla_com_br/Documents/ws-projetos-python-impressionador/automacao-web-busca-de-precos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42EEB8-E014-4F6F-8E3A-37E95301BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4B42EEB8-E014-4F6F-8E3A-37E95301BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B868CA4-D910-4FFA-BE12-5B6FB29AB716}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{CD3F9E8B-8E7C-43BA-8194-A874F6873E6D}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CD3F9E8B-8E7C-43BA-8194-A874F6873E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -57,7 +48,7 @@
     <t>rtx 3060</t>
   </si>
   <si>
-    <t>iphone 12 64gb</t>
+    <t>iphone 12 64 gb</t>
   </si>
 </sst>
 </file>
@@ -421,18 +412,18 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.578125" customWidth="1"/>
-    <col min="2" max="2" width="17.68359375" customWidth="1"/>
-    <col min="3" max="3" width="17.41796875" customWidth="1"/>
-    <col min="4" max="4" width="19.26171875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -460,7 +451,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>